<commit_message>
Final proofreading of the write up
</commit_message>
<xml_diff>
--- a/files/recipe_workbook.xlsx
+++ b/files/recipe_workbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a6b9afb2ee4a130/Documents/All_of_Maras_R/701_db/701_database_project_MaraAlexeev/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="583" documentId="8_{DBA7A22E-5743-443F-8A7D-DEE630B825BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EEBED48C-30BE-4288-99B6-0E8EEDD0D80B}"/>
+  <xr:revisionPtr revIDLastSave="594" documentId="8_{DBA7A22E-5743-443F-8A7D-DEE630B825BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EDA37325-A1C3-4577-B5D3-036FC48E0179}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="7" xr2:uid="{9A4D6EA6-92D6-4E82-8105-D38541C3CA37}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="2" activeTab="17" xr2:uid="{9A4D6EA6-92D6-4E82-8105-D38541C3CA37}"/>
   </bookViews>
   <sheets>
     <sheet name="recipe_meta" sheetId="6" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="181">
   <si>
     <t>recipe_id</t>
   </si>
@@ -223,9 +223,6 @@
   </si>
   <si>
     <t>proxy_id</t>
-  </si>
-  <si>
-    <t>Need to update recipe to correct mistake in step 8...</t>
   </si>
   <si>
     <t>Too much sauce to noodle ratio...</t>
@@ -601,6 +598,15 @@
   </si>
   <si>
     <t>Penzeys Spices</t>
+  </si>
+  <si>
+    <t>Mara's mother</t>
+  </si>
+  <si>
+    <t>Mara's maternal grandmother</t>
+  </si>
+  <si>
+    <t>Need to update recipe to correct mistake in step 2...</t>
   </si>
 </sst>
 </file>
@@ -1312,7 +1318,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1364,9 +1370,7 @@
       <c r="C2" s="9">
         <v>4</v>
       </c>
-      <c r="D2" s="11" t="s">
-        <v>8</v>
-      </c>
+      <c r="D2" s="11"/>
       <c r="E2" s="10" t="s">
         <v>40</v>
       </c>
@@ -1386,16 +1390,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="9">
+        <v>2</v>
+      </c>
+      <c r="D3" s="11"/>
+      <c r="E3" s="10" t="s">
         <v>112</v>
-      </c>
-      <c r="C3" s="9">
-        <v>2</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>113</v>
       </c>
       <c r="F3" s="9">
         <v>10</v>
@@ -1413,13 +1415,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C4">
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -1427,13 +1429,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H5">
         <v>8</v>
@@ -1451,7 +1453,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1488,7 +1490,7 @@
         <v>44127</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>57</v>
+        <v>180</v>
       </c>
       <c r="E2" s="18">
         <v>3</v>
@@ -1505,7 +1507,7 @@
         <v>44077</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E3" s="12"/>
     </row>
@@ -1520,7 +1522,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1539,22 +1541,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="F1" s="43" t="s">
+      <c r="G1" s="22" t="s">
         <v>63</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>64</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>56</v>
@@ -1580,7 +1582,7 @@
         <v>44127</v>
       </c>
       <c r="G2" s="24" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H2" s="23">
         <v>1</v>
@@ -1606,7 +1608,7 @@
         <v>44077</v>
       </c>
       <c r="G3" s="24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H3" s="23">
         <v>4</v>
@@ -1722,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
@@ -1796,10 +1798,10 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>67</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>68</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
@@ -1810,7 +1812,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -1821,7 +1823,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -1832,7 +1834,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C4" s="20"/>
       <c r="D4" s="20"/>
@@ -1843,7 +1845,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
@@ -1854,7 +1856,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
@@ -1865,7 +1867,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="12"/>
       <c r="D7" s="12"/>
@@ -1876,7 +1878,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
@@ -1884,7 +1886,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
@@ -1892,7 +1894,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
@@ -1900,7 +1902,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -1923,7 +1925,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
@@ -1964,19 +1966,19 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.45">
       <c r="A1" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>78</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.45">
@@ -1984,7 +1986,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="41" t="s">
         <v>8</v>
@@ -2001,7 +2003,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C3" s="41" t="s">
         <v>8</v>
@@ -2018,7 +2020,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" s="41" t="s">
         <v>8</v>
@@ -2035,7 +2037,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C5" s="41" t="s">
         <v>8</v>
@@ -2052,7 +2054,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="41" t="s">
         <v>8</v>
@@ -2069,7 +2071,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C7" s="41" t="s">
         <v>8</v>
@@ -2086,7 +2088,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C8" s="41" t="s">
         <v>8</v>
@@ -2121,7 +2123,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
@@ -2160,13 +2162,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>88</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>89</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
@@ -2176,10 +2178,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>90</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>91</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -2193,7 +2195,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A219B5-5360-438A-AA56-3EDC1F7D273E}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -2204,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
@@ -2245,10 +2247,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>100</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>101</v>
       </c>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
@@ -2261,7 +2263,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
@@ -2294,40 +2296,40 @@
         <v>0</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.5">
       <c r="A2" s="55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B2" s="42">
         <v>3</v>
       </c>
       <c r="C2" s="57" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="210" x14ac:dyDescent="0.45">
       <c r="A3" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" s="58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.5">
@@ -2467,7 +2469,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A16" sqref="A16:B16"/>
     </sheetView>
   </sheetViews>
@@ -2486,13 +2488,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="21" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E1" s="47"/>
       <c r="F1" s="47"/>
@@ -2511,7 +2513,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E2" s="50"/>
       <c r="F2" s="50"/>
@@ -2530,7 +2532,7 @@
         <v>2</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E3" s="50"/>
       <c r="F3" s="50"/>
@@ -2549,7 +2551,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E4" s="50"/>
       <c r="F4" s="50"/>
@@ -2568,7 +2570,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E5" s="54"/>
       <c r="F5" s="54"/>
@@ -2584,7 +2586,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.5">
@@ -2598,7 +2600,7 @@
         <v>2</v>
       </c>
       <c r="D7" s="42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.5">
@@ -2612,7 +2614,7 @@
         <v>3</v>
       </c>
       <c r="D8" s="42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.5">
@@ -2626,7 +2628,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="42" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.5">
@@ -2640,7 +2642,7 @@
         <v>1</v>
       </c>
       <c r="D10" s="42" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.5">
@@ -2654,7 +2656,7 @@
         <v>2</v>
       </c>
       <c r="D11" s="42" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.5">
@@ -2668,7 +2670,7 @@
         <v>3</v>
       </c>
       <c r="D12" s="42" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.5">
@@ -2682,7 +2684,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
@@ -2696,7 +2698,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="60" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
@@ -2710,7 +2712,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="60" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
@@ -2724,7 +2726,7 @@
         <v>3</v>
       </c>
       <c r="D16" s="60" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
   </sheetData>
@@ -2744,9 +2746,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="5" max="5" width="15.46484375" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.53125" customWidth="1"/>
+    <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="26.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" x14ac:dyDescent="0.45">
@@ -2789,13 +2794,13 @@
         <v>450</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H2" s="4"/>
     </row>
@@ -2813,7 +2818,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -2835,13 +2840,13 @@
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H4" s="4"/>
     </row>
@@ -2859,7 +2864,7 @@
         <v>100</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -2881,13 +2886,13 @@
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="20.25" x14ac:dyDescent="0.45">
@@ -2904,7 +2909,7 @@
         <v>110</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -2924,13 +2929,13 @@
         <v>120</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="20.25" x14ac:dyDescent="0.45">
@@ -2947,7 +2952,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -2967,7 +2972,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -2987,7 +2992,7 @@
         <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -3007,7 +3012,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -3027,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
@@ -3047,7 +3052,7 @@
         <v>60</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
@@ -3067,13 +3072,13 @@
         <v>60</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="20.25" x14ac:dyDescent="0.45">
@@ -3090,13 +3095,13 @@
         <v>20</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3113,13 +3118,13 @@
         <v>20</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3136,13 +3141,13 @@
         <v>150</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3159,13 +3164,13 @@
         <v>150</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F19" s="2">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3182,13 +3187,13 @@
         <v>10</v>
       </c>
       <c r="E20" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
         <v>155</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3205,13 +3210,13 @@
         <v>30</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3228,13 +3233,13 @@
         <v>20</v>
       </c>
       <c r="E22" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
         <v>158</v>
-      </c>
-      <c r="F22" s="2">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3251,13 +3256,13 @@
         <v>150</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F23" s="2">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3274,7 +3279,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F24" s="2">
         <v>1</v>
@@ -3294,7 +3299,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
@@ -3362,7 +3367,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>14</v>
@@ -3382,7 +3387,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>14</v>
@@ -3402,7 +3407,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>20</v>
@@ -3422,7 +3427,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>20</v>
@@ -3442,7 +3447,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>20</v>
@@ -3462,7 +3467,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>20</v>
@@ -3482,16 +3487,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.25" x14ac:dyDescent="0.45">
@@ -3499,16 +3504,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.25" x14ac:dyDescent="0.45">
@@ -3516,16 +3521,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.25" x14ac:dyDescent="0.45">
@@ -3533,7 +3538,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>20</v>
@@ -3550,7 +3555,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>20</v>
@@ -3567,13 +3572,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
@@ -3584,7 +3589,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>15</v>
@@ -3598,13 +3603,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.25" x14ac:dyDescent="0.45">
@@ -3612,7 +3617,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>15</v>
@@ -3626,10 +3631,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C17" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>15</v>
@@ -3643,7 +3648,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>15</v>
@@ -3657,7 +3662,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>15</v>
@@ -3671,13 +3676,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -3688,13 +3693,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="20.25" x14ac:dyDescent="0.45">
@@ -3702,7 +3707,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>15</v>
@@ -3716,13 +3721,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="60" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="20.25" x14ac:dyDescent="0.45">
@@ -3730,16 +3735,16 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
   </sheetData>
@@ -3753,7 +3758,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3781,8 +3786,8 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
+      <c r="B3" s="4">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -3869,7 +3874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB3055A9-A0D3-4226-8622-15B9EE7A1C38}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -3944,7 +3949,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -4000,7 +4005,7 @@
         <v>51</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>8</v>
+        <v>178</v>
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
@@ -4013,7 +4018,7 @@
         <v>52</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>8</v>
+        <v>179</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="36"/>

</xml_diff>

<commit_message>
Minor update to have floating toc
</commit_message>
<xml_diff>
--- a/files/recipe_workbook.xlsx
+++ b/files/recipe_workbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5a6b9afb2ee4a130/Documents/All_of_Maras_R/701_db/701_database_project_MaraAlexeev/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="594" documentId="8_{DBA7A22E-5743-443F-8A7D-DEE630B825BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{EDA37325-A1C3-4577-B5D3-036FC48E0179}"/>
+  <xr:revisionPtr revIDLastSave="846" documentId="8_{DBA7A22E-5743-443F-8A7D-DEE630B825BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F38A3333-47CB-4011-9EEE-9CED43CD5F8A}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" firstSheet="2" activeTab="17" xr2:uid="{9A4D6EA6-92D6-4E82-8105-D38541C3CA37}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="2" xr2:uid="{9A4D6EA6-92D6-4E82-8105-D38541C3CA37}"/>
   </bookViews>
   <sheets>
     <sheet name="recipe_meta" sheetId="6" r:id="rId1"/>
@@ -24,8 +24,8 @@
     <sheet name="users" sheetId="10" r:id="rId9"/>
     <sheet name="users_notes" sheetId="11" r:id="rId10"/>
     <sheet name="ratings" sheetId="12" r:id="rId11"/>
-    <sheet name="tags" sheetId="13" r:id="rId12"/>
-    <sheet name="tag_names" sheetId="14" r:id="rId13"/>
+    <sheet name="tag_names" sheetId="14" r:id="rId12"/>
+    <sheet name="tags" sheetId="13" r:id="rId13"/>
     <sheet name="tools_needed" sheetId="15" r:id="rId14"/>
     <sheet name="tool_info" sheetId="16" r:id="rId15"/>
     <sheet name="techniques_used" sheetId="17" r:id="rId16"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="206">
   <si>
     <t>recipe_id</t>
   </si>
@@ -438,9 +438,6 @@
     <t>cinnamon</t>
   </si>
   <si>
-    <t>butter</t>
-  </si>
-  <si>
     <t>flour, all purpose</t>
   </si>
   <si>
@@ -489,9 +486,6 @@
     <t>Summer &amp; Fall</t>
   </si>
   <si>
-    <t>Canned or preserved</t>
-  </si>
-  <si>
     <t>Nut</t>
   </si>
   <si>
@@ -576,9 +570,6 @@
     <t>**Salt** and **pepper** the **chicken**. Sous vide 2 hours at 140F. When done chill in an ice bath in the fridge.</t>
   </si>
   <si>
-    <t xml:space="preserve">Add cooled **chicken** to food processor. Add mayonnaise and blend until just shredded. Add **craisins** and **chopped pecans**. Stir. </t>
-  </si>
-  <si>
     <t xml:space="preserve">Season to taste with **Fox Pointe spice**. </t>
   </si>
   <si>
@@ -607,6 +598,117 @@
   </si>
   <si>
     <t>Need to update recipe to correct mistake in step 2...</t>
+  </si>
+  <si>
+    <t>Patrick Determan</t>
+  </si>
+  <si>
+    <t>Bread</t>
+  </si>
+  <si>
+    <t>No Knead Bread</t>
+  </si>
+  <si>
+    <t>https://cooking.nytimes.com/recipes/11376-no-knead-bread</t>
+  </si>
+  <si>
+    <t>Jim Lahey</t>
+  </si>
+  <si>
+    <t>Owner of Sullivan Street Bakery</t>
+  </si>
+  <si>
+    <t>Mara's go to bread.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combine **flour**, **salt**, and **yeast** in a bowl. Add **water**, which should be 105F. Stir to blend. Cover bowl with plastic wrap. Let dough rest at least 12 hours at roughly 70F. </t>
+  </si>
+  <si>
+    <t>Lightly flour a surface to work with dough. Sprinkle dough with small amount of flour. Fold dough over on itself twice. Cover loosely with plastic wrap and let rest 15 minutes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coat hands with small amount of flour to prevent dough from sticking. Dust two cotton towels with flour.  Gently shape dough into ball. Place dough seam side down on  cotton towel. Dust dough again with flour, cover with other towel. Allow to rise at room temperature for 120 minutes. Dough should double in size. </t>
+  </si>
+  <si>
+    <t>At 90 minute mark, turn oven on to 450F and place a Dutch oven, base and lid, in the oven to heat as well.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At 120 minute mark, remove the base of the Dutch oven, coat the bottom with **cornmeal** and then place dough into the base seam side up. Sprinkle or spray a small amount of water on the dough. Slash the top of the bread. Place in oven and then cover the Dutch oven with its lid. Bake covered for 30 minutes. At the 30 minute mark, remove the lid and back another 15 to 30 minutes until loaf is nicely brown. Remove base of Dutch oven from oven. Carefully, remove bread from base, and allow to cool on a rack. </t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t>active dry yeast</t>
+  </si>
+  <si>
+    <t>cornmeal</t>
+  </si>
+  <si>
+    <t>at 105F</t>
+  </si>
+  <si>
+    <t>mayonnaise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add cooled **chicken** to food processor. Add mayonnaise and blend until just shredded. Add **dried cranberries** and **chopped pecans**. Stir. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Melt **butter** and **chocolate** together using a double boiler, stir frequently. When well combined, add **salt** and stir. </t>
+  </si>
+  <si>
+    <t>Add **evaporated milk** to mixture. Stirring frequently with whisk, heat sauce until it is velvety smooth.</t>
+  </si>
+  <si>
+    <t>Stir **sugar** into mixture 15 grams at a time and incorporate well before adding more sugar. </t>
+  </si>
+  <si>
+    <t>baking chocolate</t>
+  </si>
+  <si>
+    <t>butter, unsalted</t>
+  </si>
+  <si>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>evaporated milk</t>
+  </si>
+  <si>
+    <t>Olivier Salad</t>
+  </si>
+  <si>
+    <t>Olivier salad, or salat Olivier, is a traditional Russian dish often served around New Years. This is our family version of this popular dish. Most families do have their own version of the recipe, which is of course the correct version of the recipe.</t>
+  </si>
+  <si>
+    <t>1 cup mayo
+1.5 tbsp mustard
+1/2 lb bologna or mortadella
+1/2 small onion, diced (3 oz)
+1 15 oz can peas drained (but not rinsed)
+1 large or 2 small cucumbers, peeled and seeded (6 oz)
+5 eggs, hard boiled (8 oz)
+2 large carrots, peeled (9 oz)
+5 small potatoes (usually yukon gold) (1 lb)
+1/2 lb chicken breast (skinless, boneless)
+"Our" salat Olivier (Olivier salad) recipe:
+Gather all of the ingredients below (some require preparation, as indicated) and dice them into similarly sized pieces, ranging from a 1 cm2 slice of mortadella to a pea's size to about 1cm3 piece of potato.
+Then mix everything up and chill.
+1 cup mayo
+1.5tbsp mustard
+1/2 lb bologna or mortadella
+1/2 small onion, diced
+1 can peas
+1 large or 2 small cucumbers, peeled and seeded
+Hard-boil (11 minutes at simmer and chill in ice bath, peel, then dice): 5 eggs
+Boil water, add lots of salt, and then simmer these for 20 minutes ( ~10 minutes for the carrots) on medium-low heat (and then chill):
+2 large carrots, peeled
+5 small potatoes (usually yukon gold, can peel or leave unpeeled based on perference)
+Boil water, add some salt, and then simmer covered for 10--15 minutes until cooked through (and then chill) or in sous vide for 2 hours at 135F:
+1/2 lb chicken breast (skinless, boneless)
+Remark: with the exception of the salt involved in boiling, this recipe calls for no salt or pepper. We typically leave the salting/peppering to the individual 
+Yield: 10 US cups (2.5--3 big deli cups)
+Serves: 10ish = 4 people twice and then a little?</t>
   </si>
 </sst>
 </file>
@@ -811,7 +913,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -834,11 +936,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1000,6 +1122,15 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1314,11 +1445,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC17A43C-FFC5-464F-9BEB-4729478DC9F4}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D3"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1326,7 +1457,7 @@
     <col min="1" max="1" width="13.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.86328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.53125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.3984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.265625" bestFit="1" customWidth="1"/>
@@ -1423,22 +1554,74 @@
       <c r="E4" t="s">
         <v>114</v>
       </c>
+      <c r="F4">
+        <v>45</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>20</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H5">
         <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>181</v>
+      </c>
+      <c r="E6" t="s">
+        <v>184</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6">
+        <v>900</v>
+      </c>
+      <c r="H6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>204</v>
+      </c>
+      <c r="H7">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1490,7 +1673,7 @@
         <v>44127</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E2" s="18">
         <v>3</v>
@@ -1710,6 +1893,141 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BC439B-56CB-45EC-9BC2-95AA8F75A564}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="35.265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+    </row>
+    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A3" s="18">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+    </row>
+    <row r="4" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A4" s="18">
+        <v>3</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A5" s="18">
+        <v>4</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+    </row>
+    <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A6" s="18">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+    </row>
+    <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="18">
+        <v>6</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A8" s="18">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A9" s="18">
+        <v>8</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A10" s="18">
+        <v>9</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A11" s="18">
+        <v>10</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
+      <c r="A12" s="18">
+        <v>11</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3977833A-D0A4-47F6-AAC8-226453DAB85C}">
   <dimension ref="A1:E7"/>
   <sheetViews>
@@ -1779,130 +2097,6 @@
       </c>
       <c r="B7">
         <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07BC439B-56CB-45EC-9BC2-95AA8F75A564}">
-  <dimension ref="A1:E11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A1" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-    </row>
-    <row r="2" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A2" s="18">
-        <v>1</v>
-      </c>
-      <c r="B2" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="18">
-        <v>2</v>
-      </c>
-      <c r="B3" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="4" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A4" s="18">
-        <v>3</v>
-      </c>
-      <c r="B4" s="19" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-    </row>
-    <row r="5" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A5" s="18">
-        <v>4</v>
-      </c>
-      <c r="B5" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A6" s="18">
-        <v>5</v>
-      </c>
-      <c r="B6" s="19" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A7" s="18">
-        <v>6</v>
-      </c>
-      <c r="B7" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-    </row>
-    <row r="8" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="18">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A9" s="18">
-        <v>8</v>
-      </c>
-      <c r="B9" s="19" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A10" s="18">
-        <v>9</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="17.25" x14ac:dyDescent="0.45">
-      <c r="A11" s="18">
-        <v>10</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -2195,7 +2389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57A219B5-5360-438A-AA56-3EDC1F7D273E}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
@@ -2279,7 +2473,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2323,17 +2517,25 @@
     </row>
     <row r="4" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
       <c r="C4" s="59" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="C5" s="49"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="409.5" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" s="49" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="C6" s="49"/>
@@ -2466,11 +2668,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED0582FD-8CF0-4F52-ADF4-94EEA7D2405F}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A16" sqref="A16:B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -2684,7 +2886,7 @@
         <v>4</v>
       </c>
       <c r="D13" s="42" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.5">
@@ -2698,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="D14" s="60" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.5">
@@ -2712,7 +2914,7 @@
         <v>2</v>
       </c>
       <c r="D15" s="60" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.5">
@@ -2726,7 +2928,119 @@
         <v>3</v>
       </c>
       <c r="D16" s="60" t="s">
-        <v>171</v>
+        <v>168</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A17" s="42">
+        <v>5</v>
+      </c>
+      <c r="B17" s="42">
+        <v>1</v>
+      </c>
+      <c r="C17" s="42">
+        <v>1</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A18" s="42">
+        <v>5</v>
+      </c>
+      <c r="B18" s="42">
+        <v>1</v>
+      </c>
+      <c r="C18" s="42">
+        <v>2</v>
+      </c>
+      <c r="D18" s="42" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A19" s="42">
+        <v>5</v>
+      </c>
+      <c r="B19" s="42">
+        <v>1</v>
+      </c>
+      <c r="C19" s="42">
+        <v>3</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A20" s="42">
+        <v>5</v>
+      </c>
+      <c r="B20" s="42">
+        <v>1</v>
+      </c>
+      <c r="C20" s="42">
+        <v>4</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A21" s="42">
+        <v>5</v>
+      </c>
+      <c r="B21" s="42">
+        <v>1</v>
+      </c>
+      <c r="C21" s="42">
+        <v>5</v>
+      </c>
+      <c r="D21" s="42" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A22" s="42">
+        <v>3</v>
+      </c>
+      <c r="B22" s="42">
+        <v>1</v>
+      </c>
+      <c r="C22" s="42">
+        <v>1</v>
+      </c>
+      <c r="D22" s="42" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A23" s="42">
+        <v>3</v>
+      </c>
+      <c r="B23" s="42">
+        <v>1</v>
+      </c>
+      <c r="C23" s="42">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A24" s="42">
+        <v>3</v>
+      </c>
+      <c r="B24" s="42">
+        <v>1</v>
+      </c>
+      <c r="C24" s="42">
+        <v>3</v>
+      </c>
+      <c r="D24" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2737,11 +3051,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D41A8F-8DA3-4347-B84B-C79737C37A93}">
-  <dimension ref="A1:H28"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2794,7 +3108,7 @@
         <v>450</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
@@ -2818,7 +3132,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -2840,7 +3154,7 @@
         <v>6</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F4" s="2">
         <v>1</v>
@@ -2864,7 +3178,7 @@
         <v>100</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F5" s="2">
         <v>1</v>
@@ -2886,7 +3200,7 @@
         <v>3</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -2909,7 +3223,7 @@
         <v>110</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F7" s="2">
         <v>1</v>
@@ -2929,7 +3243,7 @@
         <v>120</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F8" s="2">
         <v>1</v>
@@ -2952,7 +3266,7 @@
         <v>30</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F9" s="2">
         <v>1</v>
@@ -2972,7 +3286,7 @@
         <v>15</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F10" s="2">
         <v>1</v>
@@ -2992,7 +3306,7 @@
         <v>30</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F11" s="2">
         <v>1</v>
@@ -3012,7 +3326,7 @@
         <v>1</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F12" s="2">
         <v>1</v>
@@ -3032,7 +3346,7 @@
         <v>1</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F13" s="2">
         <v>1</v>
@@ -3052,7 +3366,7 @@
         <v>60</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F14" s="2">
         <v>1</v>
@@ -3072,13 +3386,13 @@
         <v>60</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F15" s="2">
         <v>1</v>
       </c>
       <c r="G15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="20.25" x14ac:dyDescent="0.45">
@@ -3095,13 +3409,13 @@
         <v>20</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F16" s="2">
         <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3118,13 +3432,13 @@
         <v>20</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F17" s="2">
         <v>1</v>
       </c>
       <c r="G17" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3141,13 +3455,13 @@
         <v>150</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
       </c>
       <c r="G18" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3164,13 +3478,13 @@
         <v>150</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F19" s="2">
         <v>1</v>
       </c>
       <c r="G19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3187,13 +3501,13 @@
         <v>10</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3210,13 +3524,13 @@
         <v>30</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F21" s="2">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3233,13 +3547,13 @@
         <v>20</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F22" s="2">
         <v>1</v>
       </c>
       <c r="G22" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3256,13 +3570,13 @@
         <v>150</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F23" s="2">
         <v>1</v>
       </c>
       <c r="G23" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
@@ -3279,7 +3593,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F24" s="2">
         <v>1</v>
@@ -3299,7 +3613,7 @@
         <v>1</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F25" s="2">
         <v>1</v>
@@ -3309,15 +3623,386 @@
       <c r="A26" s="2">
         <v>4</v>
       </c>
+      <c r="B26">
+        <v>10</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>6</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <v>4</v>
       </c>
+      <c r="B27">
+        <v>11</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1</v>
+      </c>
+      <c r="D27" s="2">
+        <v>6</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <v>4</v>
+      </c>
+      <c r="B28">
+        <v>22</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1</v>
+      </c>
+      <c r="D28" s="2">
+        <v>300</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A29" s="2">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>27</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2">
+        <v>80</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A30" s="2">
+        <v>4</v>
+      </c>
+      <c r="B30">
+        <v>20</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>60</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A31" s="2">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>19</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2">
+        <v>50</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31" s="2">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A32" s="2">
+        <v>4</v>
+      </c>
+      <c r="B32">
+        <v>23</v>
+      </c>
+      <c r="C32" s="2">
+        <v>3</v>
+      </c>
+      <c r="D32" s="2">
+        <v>6</v>
+      </c>
+      <c r="E32" t="s">
+        <v>155</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A33" s="2">
+        <v>5</v>
+      </c>
+      <c r="B33">
+        <v>6</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>900</v>
+      </c>
+      <c r="E33" t="s">
+        <v>155</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A34" s="2">
+        <v>5</v>
+      </c>
+      <c r="B34">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>17</v>
+      </c>
+      <c r="E34" t="s">
+        <v>155</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A35" s="2">
+        <v>5</v>
+      </c>
+      <c r="B35">
+        <v>25</v>
+      </c>
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>155</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A36" s="2">
+        <v>5</v>
+      </c>
+      <c r="B36">
+        <v>24</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>680</v>
+      </c>
+      <c r="E36" t="s">
+        <v>155</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A37" s="2">
+        <v>5</v>
+      </c>
+      <c r="B37">
+        <v>6</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>5</v>
+      </c>
+      <c r="E37" t="s">
+        <v>155</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A38" s="2">
+        <v>5</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>3</v>
+      </c>
+      <c r="D38">
+        <v>5</v>
+      </c>
+      <c r="E38" t="s">
+        <v>155</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A39" s="2">
+        <v>5</v>
+      </c>
+      <c r="B39">
+        <v>26</v>
+      </c>
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>10</v>
+      </c>
+      <c r="E39" t="s">
+        <v>155</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A40" s="2">
+        <v>3</v>
+      </c>
+      <c r="B40">
+        <v>5</v>
+      </c>
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40">
+        <v>110</v>
+      </c>
+      <c r="E40" t="s">
+        <v>155</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A41" s="2">
+        <v>3</v>
+      </c>
+      <c r="B41">
+        <v>28</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41">
+        <v>250</v>
+      </c>
+      <c r="E41" t="s">
+        <v>155</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A42">
+        <v>3</v>
+      </c>
+      <c r="B42">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>1</v>
+      </c>
+      <c r="E42" t="s">
+        <v>155</v>
+      </c>
+      <c r="F42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A43" s="2">
+        <v>3</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>600</v>
+      </c>
+      <c r="E43" t="s">
+        <v>155</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A44" s="2">
+        <v>3</v>
+      </c>
+      <c r="B44">
+        <v>29</v>
+      </c>
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>350</v>
+      </c>
+      <c r="E44" t="s">
+        <v>146</v>
+      </c>
+      <c r="F44">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -3328,10 +4013,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8A2811-654B-4F43-B867-8B5BD8C350AE}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3447,7 +4132,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>124</v>
+        <v>200</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>20</v>
@@ -3467,7 +4152,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>20</v>
@@ -3487,16 +4172,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="20.25" x14ac:dyDescent="0.45">
@@ -3504,7 +4189,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>20</v>
@@ -3513,7 +4198,7 @@
         <v>119</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="20.25" x14ac:dyDescent="0.45">
@@ -3521,16 +4206,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="20.25" x14ac:dyDescent="0.45">
@@ -3538,7 +4223,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>20</v>
@@ -3555,7 +4240,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>20</v>
@@ -3572,13 +4257,13 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E13" t="s">
         <v>22</v>
@@ -3589,7 +4274,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>15</v>
@@ -3603,13 +4288,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>141</v>
+        <v>132</v>
+      </c>
+      <c r="D15" t="s">
+        <v>144</v>
       </c>
       <c r="E15" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="20.25" x14ac:dyDescent="0.45">
@@ -3617,7 +4302,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>15</v>
@@ -3631,10 +4316,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>15</v>
@@ -3648,7 +4333,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>15</v>
@@ -3662,7 +4347,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>15</v>
@@ -3676,13 +4361,13 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C20" t="s">
         <v>20</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -3693,13 +4378,13 @@
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="20.25" x14ac:dyDescent="0.45">
@@ -3707,7 +4392,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>15</v>
@@ -3721,13 +4406,13 @@
         <v>22</v>
       </c>
       <c r="B23" s="60" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="20.25" x14ac:dyDescent="0.45">
@@ -3735,16 +4420,118 @@
         <v>23</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C24" t="s">
         <v>20</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C26" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C28" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="20.25" x14ac:dyDescent="0.45">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -3946,16 +4733,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EBB52D3-0EA7-49C6-9FAA-D8419F48B9E9}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" x14ac:dyDescent="0.45">
@@ -3991,9 +4778,7 @@
       <c r="B3" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="34" t="s">
-        <v>8</v>
-      </c>
+      <c r="C3" s="34"/>
       <c r="D3" s="35"/>
       <c r="E3" s="35"/>
     </row>
@@ -4005,7 +4790,7 @@
         <v>51</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D4" s="35"/>
       <c r="E4" s="35"/>
@@ -4018,10 +4803,29 @@
         <v>52</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="D5" s="36"/>
       <c r="E5" s="36"/>
+    </row>
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.45">
+      <c r="A6" s="61">
+        <v>5</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.45">
+      <c r="A7" s="61">
+        <v>6</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" s="63" t="s">
+        <v>183</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>